<commit_message>
Adding comments and create outputs
</commit_message>
<xml_diff>
--- a/Outputs/parameters.xlsx
+++ b/Outputs/parameters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -618,66 +618,134 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Battery Capacity</t>
+          <t>Payload Width</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>33.800000000000004</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Ah</t>
+          <t>m</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Battery Cells</t>
+          <t>Payload Length</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>m</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Motor Name</t>
+          <t>Payload Height</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SunnySky X Series V3 X2220 KV2200</t>
+          <t>0.2</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>m</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
+          <t>Payload Weight</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>19.6133</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Battery Capacity</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>28.6</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ah</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Battery Cells</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>Motor Name</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SunnySky X Series V3 X2220 KV2200</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
           <t>Lift to Drag (design point)</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>13.610057933566454</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11.741207493829714</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>nan</t>
         </is>

</xml_diff>